<commit_message>
update PQT calc and Spain data
 non-self isolation calculation was updated such that if symptoms appear in quarantine the individual does isolate
</commit_message>
<xml_diff>
--- a/Country_Data/Destination_Spain-2019.xlsx
+++ b/Country_Data/Destination_Spain-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Sufficient-strategies-for-travel-quarantine-and-testing\Country_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9984316-439E-4759-91E3-5B294708603D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D24101-2D76-4B67-80BB-7F0C653DD31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24765" yWindow="6435" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2880" yWindow="5520" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>European Countries - Nights and arrivals - Annual data</t>
   </si>
@@ -66,7 +66,28 @@
     <t>Destination: Spain</t>
   </si>
   <si>
-    <t>Information: excel file (duration of stay is the avg of the 12 months)</t>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Republic of Ireland</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Information: excel file (duration of stay is the avg of the 12 months) and from the PDF for Spain (Scaled by rented accomodations)</t>
   </si>
 </sst>
 </file>
@@ -226,10 +247,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -582,7 +603,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J4"/>
+      <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -637,32 +658,32 @@
       <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="A4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -714,14 +735,19 @@
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>11147228.200000001</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>D8*(68314398/83701011)</f>
+        <v>9121979.941137271</v>
+      </c>
+      <c r="D8" s="6">
+        <v>11176545</v>
+      </c>
+      <c r="E8" s="6">
+        <f>H8*B8</f>
+        <v>28088475.615367394</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7">
@@ -732,14 +758,19 @@
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9">
-        <v>11161236.198100001</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B17" si="0">D9*(68314398/83701011)</f>
+        <v>2072120.4282698808</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2538829</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" ref="E9:E17" si="1">H9*B9</f>
+        <v>6380490.2550911382</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
       <c r="H9" s="7">
@@ -750,14 +781,19 @@
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9">
-        <v>18004157.8189</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9105759.3444009665</v>
+      </c>
+      <c r="D10" s="9">
+        <v>11156671</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="1"/>
+        <v>28038529.02056732</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
       <c r="H10" s="7">
@@ -767,86 +803,163 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1776892.3456872941</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2177106</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="1"/>
+        <v>5471421.5164945843</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>3707630.6118235779</v>
+      </c>
+      <c r="D12" s="9">
+        <v>4542709</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="1"/>
+        <v>11416566.655814461</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>3021421.9967989638</v>
+      </c>
+      <c r="D13" s="9">
+        <v>3701944</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="1"/>
+        <v>9303587.4479506407</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1992067.8575902507</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2440746</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="1"/>
+        <v>6133991.7214403385</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>14754814.358673016</v>
+      </c>
+      <c r="D15" s="9">
+        <v>18078076</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="1"/>
+        <v>45433145.65447174</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1489381.9828761925</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1824839</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="1"/>
+        <v>4586117.2440563114</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1070609.987242663</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1311746</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="1"/>
+        <v>3296631.0728902058</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7">
+        <v>3.0792082197744302</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>

</xml_diff>